<commit_message>
fix: correcao do nome no email para conter nome do mes em pt-br
</commit_message>
<xml_diff>
--- a/Output/Relatorio-Erros-DE767565.xlsx
+++ b/Output/Relatorio-Erros-DE767565.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\levi.sistemas\Downloads\NuCase\NubankCase_RelatorioVendas\Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F1A212E-D557-4FBB-BA35-2A730792A547}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16F92735-3AC2-423F-BE9E-7B47098DDAA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{402E8141-2EC6-4914-8F80-B5BF27F87689}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{742104B5-4D75-41F6-985E-A04CE0313301}"/>
   </bookViews>
   <sheets>
     <sheet name="Erros" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>INVOICE</t>
   </si>
@@ -46,9 +46,6 @@
   </si>
   <si>
     <t>Erros Encontrados</t>
-  </si>
-  <si>
-    <t>DE767565</t>
   </si>
 </sst>
 </file>
@@ -419,8 +416,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6FDC33C-48E0-4702-9BA2-02B8FFD38846}">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F05E6982-EB73-4737-8D65-32E18AB9CEF6}">
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -437,21 +434,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>663318</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A48932E3-19DB-4BC2-93C4-A59B2DECA103}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CB4B487-BB17-4184-B46A-180A39A6BB8E}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>